<commit_message>
test P7 with -10 percent
</commit_message>
<xml_diff>
--- a/results/I2_N10_T100_C275_0_P2_res.xlsx
+++ b/results/I2_N10_T100_C275_0_P2_res.xlsx
@@ -473,7 +473,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>976.1856520136134</v>
+        <v>56.63098846897222</v>
       </c>
     </row>
     <row r="4">
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.02300000190734863</v>
+        <v>0.01900005340576172</v>
       </c>
     </row>
     <row r="5">
@@ -503,7 +503,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>32.40565201361344</v>
+        <v>38.17098846897686</v>
       </c>
     </row>
     <row r="7">
@@ -513,7 +513,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2.733406698459491</v>
+        <v>0.6217041096856285</v>
       </c>
     </row>
     <row r="8">
@@ -523,7 +523,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2.733406698459491</v>
+        <v>0.6217041096856285</v>
       </c>
     </row>
     <row r="9">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>779.4</v>
+        <v>18.45999999999535</v>
       </c>
     </row>
     <row r="10">
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>164.38</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -557,7 +557,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -584,89 +584,12 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>2</v>
-      </c>
-      <c r="C3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>3</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="n">
-        <v>4</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" t="n">
-        <v>5</v>
-      </c>
-      <c r="C9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -722,7 +645,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" t="n">
         <v>1</v>
@@ -755,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C6" t="n">
         <v>1</v>
@@ -766,7 +689,7 @@
         <v>3</v>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="C7" t="n">
         <v>1</v>
@@ -788,7 +711,7 @@
         <v>5</v>
       </c>
       <c r="B9" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C9" t="n">
         <v>1</v>
@@ -799,7 +722,7 @@
         <v>6</v>
       </c>
       <c r="B10" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C10" t="n">
         <v>1</v>
@@ -832,7 +755,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="n">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="C13" t="n">
         <v>1</v>
@@ -843,7 +766,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C14" t="n">
         <v>1</v>
@@ -890,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -1072,7 +995,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>5.336665625650539</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
@@ -1080,7 +1003,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>38.91304018828278</v>
+        <v>34.3488504228129</v>
       </c>
     </row>
     <row r="5">
@@ -1088,7 +1011,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>30.34885527085025</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
@@ -1096,7 +1019,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>30</v>
+        <v>35.00919155153804</v>
       </c>
     </row>
     <row r="7">
@@ -1104,7 +1027,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>35.54177106295361</v>
+        <v>37.06506101847738</v>
       </c>
     </row>
     <row r="8">
@@ -1120,7 +1043,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>30</v>
+        <v>30.60033324079214</v>
       </c>
     </row>
     <row r="10">
@@ -1128,7 +1051,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>32.31224998648503</v>
+        <v>37.32144153802307</v>
       </c>
     </row>
     <row r="11">
@@ -1136,7 +1059,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>34.76592070603971</v>
+        <v>39.77511225757775</v>
       </c>
     </row>
     <row r="12">
@@ -1144,7 +1067,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>32.01159140980467</v>
+        <v>32.61192465059682</v>
       </c>
     </row>
     <row r="13">
@@ -1152,7 +1075,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>32.66758337047729</v>
+        <v>36.71671453559702</v>
       </c>
     </row>
     <row r="14">
@@ -1160,7 +1083,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>41.49352463892379</v>
+        <v>38.25017704655227</v>
       </c>
     </row>
     <row r="15">
@@ -1168,7 +1091,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>36.7268870910285</v>
+        <v>42.88363280600589</v>
       </c>
     </row>
   </sheetData>
@@ -1182,7 +1105,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1214,113 +1137,15 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>12</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>12</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>5</v>
-      </c>
-      <c r="B5" t="n">
-        <v>13</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>13</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>13</v>
-      </c>
-      <c r="C7" t="n">
-        <v>3</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="n">
-        <v>13</v>
-      </c>
-      <c r="C8" t="n">
-        <v>4</v>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" t="n">
-        <v>13</v>
-      </c>
-      <c r="C9" t="n">
-        <v>5</v>
-      </c>
-      <c r="D9" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1423,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>97.1700000000008</v>
+        <v>109.9450000000008</v>
       </c>
     </row>
     <row r="8">
@@ -1434,7 +1259,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>99.27000000000081</v>
+        <v>117.5900000000008</v>
       </c>
     </row>
     <row r="9">
@@ -1445,7 +1270,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>100.1150000000008</v>
+        <v>113.2700000000008</v>
       </c>
     </row>
     <row r="10">
@@ -1456,7 +1281,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>99.0400000000008</v>
+        <v>119.1550000000008</v>
       </c>
     </row>
     <row r="11">
@@ -1467,7 +1292,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>97.9800000000008</v>
+        <v>115.8050000000008</v>
       </c>
     </row>
     <row r="12">
@@ -1478,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>307.515</v>
+        <v>188.8550000000006</v>
       </c>
     </row>
     <row r="13">
@@ -1489,7 +1314,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>327.86</v>
+        <v>192.9200000000006</v>
       </c>
     </row>
     <row r="14">
@@ -1500,7 +1325,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>306.57</v>
+        <v>178.5050000000006</v>
       </c>
     </row>
     <row r="15">
@@ -1511,7 +1336,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>318.89</v>
+        <v>189.2700000000006</v>
       </c>
     </row>
     <row r="16">
@@ -1522,7 +1347,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>311.82</v>
+        <v>182.1250000000006</v>
       </c>
     </row>
     <row r="17">
@@ -1533,7 +1358,7 @@
         <v>1</v>
       </c>
       <c r="C17" t="n">
-        <v>154.3</v>
+        <v>46.91999999999942</v>
       </c>
     </row>
     <row r="18">
@@ -1544,7 +1369,7 @@
         <v>2</v>
       </c>
       <c r="C18" t="n">
-        <v>148.3449999999993</v>
+        <v>36.10499999999942</v>
       </c>
     </row>
     <row r="19">
@@ -1555,7 +1380,7 @@
         <v>3</v>
       </c>
       <c r="C19" t="n">
-        <v>128.7049999999993</v>
+        <v>34.91499999999942</v>
       </c>
     </row>
     <row r="20">
@@ -1566,7 +1391,7 @@
         <v>4</v>
       </c>
       <c r="C20" t="n">
-        <v>146.3249999999993</v>
+        <v>37.48999999999942</v>
       </c>
     </row>
     <row r="21">
@@ -1577,7 +1402,7 @@
         <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>134.2149999999993</v>
+        <v>39.43499999999941</v>
       </c>
     </row>
     <row r="22">
@@ -1588,7 +1413,7 @@
         <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>72.6299999999995</v>
+        <v>119.55</v>
       </c>
     </row>
     <row r="23">
@@ -1599,7 +1424,7 @@
         <v>2</v>
       </c>
       <c r="C23" t="n">
-        <v>80.0549999999995</v>
+        <v>116.1599999999989</v>
       </c>
     </row>
     <row r="24">
@@ -1610,7 +1435,7 @@
         <v>3</v>
       </c>
       <c r="C24" t="n">
-        <v>82.31999999999948</v>
+        <v>117.2349999999989</v>
       </c>
     </row>
     <row r="25">
@@ -1621,7 +1446,7 @@
         <v>4</v>
       </c>
       <c r="C25" t="n">
-        <v>83.9549999999995</v>
+        <v>121.4449999999989</v>
       </c>
     </row>
     <row r="26">
@@ -1632,7 +1457,7 @@
         <v>5</v>
       </c>
       <c r="C26" t="n">
-        <v>80.8149999999995</v>
+        <v>120.25</v>
       </c>
     </row>
     <row r="27">
@@ -1643,7 +1468,7 @@
         <v>1</v>
       </c>
       <c r="C27" t="n">
-        <v>308.075</v>
+        <v>258.7350000000008</v>
       </c>
     </row>
     <row r="28">
@@ -1654,7 +1479,7 @@
         <v>2</v>
       </c>
       <c r="C28" t="n">
-        <v>318.99</v>
+        <v>269.2400000000008</v>
       </c>
     </row>
     <row r="29">
@@ -1665,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="n">
-        <v>312.23</v>
+        <v>250.9150000000008</v>
       </c>
     </row>
     <row r="30">
@@ -1676,7 +1501,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>322.11</v>
+        <v>261.9150000000008</v>
       </c>
     </row>
     <row r="31">
@@ -1687,7 +1512,7 @@
         <v>5</v>
       </c>
       <c r="C31" t="n">
-        <v>305.64</v>
+        <v>255.0150000000008</v>
       </c>
     </row>
     <row r="32">
@@ -1753,7 +1578,7 @@
         <v>1</v>
       </c>
       <c r="C37" t="n">
-        <v>180.2450000000005</v>
+        <v>193.0200000000017</v>
       </c>
     </row>
     <row r="38">
@@ -1764,7 +1589,7 @@
         <v>2</v>
       </c>
       <c r="C38" t="n">
-        <v>183.9900000000005</v>
+        <v>202.3100000000017</v>
       </c>
     </row>
     <row r="39">
@@ -1775,7 +1600,7 @@
         <v>3</v>
       </c>
       <c r="C39" t="n">
-        <v>178.0900000000005</v>
+        <v>191.2450000000017</v>
       </c>
     </row>
     <row r="40">
@@ -1786,7 +1611,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>188.8100000000005</v>
+        <v>208.9250000000017</v>
       </c>
     </row>
     <row r="41">
@@ -1797,7 +1622,7 @@
         <v>5</v>
       </c>
       <c r="C41" t="n">
-        <v>179.8350000000005</v>
+        <v>197.6600000000017</v>
       </c>
     </row>
     <row r="42">
@@ -1808,7 +1633,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>140.5549999999995</v>
+        <v>187.4749999999983</v>
       </c>
     </row>
     <row r="43">
@@ -1819,7 +1644,7 @@
         <v>2</v>
       </c>
       <c r="C43" t="n">
-        <v>159.2149999999995</v>
+        <v>195.3199999999983</v>
       </c>
     </row>
     <row r="44">
@@ -1830,7 +1655,7 @@
         <v>3</v>
       </c>
       <c r="C44" t="n">
-        <v>142.1399999999987</v>
+        <v>177.0549999999983</v>
       </c>
     </row>
     <row r="45">
@@ -1841,7 +1666,7 @@
         <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>147.7249999999995</v>
+        <v>185.2149999999984</v>
       </c>
     </row>
     <row r="46">
@@ -1852,7 +1677,7 @@
         <v>5</v>
       </c>
       <c r="C46" t="n">
-        <v>139.7449999999988</v>
+        <v>179.1799999999983</v>
       </c>
     </row>
     <row r="47">
@@ -1863,7 +1688,7 @@
         <v>1</v>
       </c>
       <c r="C47" t="n">
-        <v>226.04</v>
+        <v>272.9599999999988</v>
       </c>
     </row>
     <row r="48">
@@ -1874,7 +1699,7 @@
         <v>2</v>
       </c>
       <c r="C48" t="n">
-        <v>247.18</v>
+        <v>283.2849999999988</v>
       </c>
     </row>
     <row r="49">
@@ -1885,7 +1710,7 @@
         <v>3</v>
       </c>
       <c r="C49" t="n">
-        <v>221.8549999999993</v>
+        <v>256.7699999999988</v>
       </c>
     </row>
     <row r="50">
@@ -1896,7 +1721,7 @@
         <v>4</v>
       </c>
       <c r="C50" t="n">
-        <v>238.455</v>
+        <v>275.9449999999989</v>
       </c>
     </row>
     <row r="51">
@@ -1907,7 +1732,7 @@
         <v>5</v>
       </c>
       <c r="C51" t="n">
-        <v>224.4749999999993</v>
+        <v>263.9099999999988</v>
       </c>
     </row>
     <row r="52">
@@ -1918,7 +1743,7 @@
         <v>1</v>
       </c>
       <c r="C52" t="n">
-        <v>238.1949999999998</v>
+        <v>250.970000000001</v>
       </c>
     </row>
     <row r="53">
@@ -1929,7 +1754,7 @@
         <v>2</v>
       </c>
       <c r="C53" t="n">
-        <v>242.6699999999998</v>
+        <v>260.9900000000009</v>
       </c>
     </row>
     <row r="54">
@@ -1940,7 +1765,7 @@
         <v>3</v>
       </c>
       <c r="C54" t="n">
-        <v>239.8199999999998</v>
+        <v>252.975000000001</v>
       </c>
     </row>
     <row r="55">
@@ -1951,7 +1776,7 @@
         <v>4</v>
       </c>
       <c r="C55" t="n">
-        <v>249.4649999999998</v>
+        <v>269.580000000001</v>
       </c>
     </row>
     <row r="56">
@@ -1962,7 +1787,7 @@
         <v>5</v>
       </c>
       <c r="C56" t="n">
-        <v>232.75</v>
+        <v>250.575000000001</v>
       </c>
     </row>
     <row r="57">
@@ -1973,7 +1798,7 @@
         <v>1</v>
       </c>
       <c r="C57" t="n">
-        <v>154.3</v>
+        <v>250.970000000001</v>
       </c>
     </row>
     <row r="58">
@@ -1984,7 +1809,7 @@
         <v>2</v>
       </c>
       <c r="C58" t="n">
-        <v>148.3449999999993</v>
+        <v>260.9900000000009</v>
       </c>
     </row>
     <row r="59">
@@ -1995,7 +1820,7 @@
         <v>3</v>
       </c>
       <c r="C59" t="n">
-        <v>128.7049999999993</v>
+        <v>252.975000000001</v>
       </c>
     </row>
     <row r="60">
@@ -2006,7 +1831,7 @@
         <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>146.3249999999993</v>
+        <v>269.580000000001</v>
       </c>
     </row>
     <row r="61">
@@ -2017,7 +1842,7 @@
         <v>5</v>
       </c>
       <c r="C61" t="n">
-        <v>134.2149999999993</v>
+        <v>250.575000000001</v>
       </c>
     </row>
     <row r="62">
@@ -2028,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>307.515</v>
+        <v>258.7350000000008</v>
       </c>
     </row>
     <row r="63">
@@ -2039,7 +1864,7 @@
         <v>2</v>
       </c>
       <c r="C63" t="n">
-        <v>327.86</v>
+        <v>269.2400000000008</v>
       </c>
     </row>
     <row r="64">
@@ -2050,7 +1875,7 @@
         <v>3</v>
       </c>
       <c r="C64" t="n">
-        <v>306.57</v>
+        <v>250.9150000000008</v>
       </c>
     </row>
     <row r="65">
@@ -2061,7 +1886,7 @@
         <v>4</v>
       </c>
       <c r="C65" t="n">
-        <v>318.89</v>
+        <v>261.9150000000008</v>
       </c>
     </row>
     <row r="66">
@@ -2072,7 +1897,7 @@
         <v>5</v>
       </c>
       <c r="C66" t="n">
-        <v>311.82</v>
+        <v>255.0150000000008</v>
       </c>
     </row>
     <row r="67">
@@ -2083,7 +1908,7 @@
         <v>1</v>
       </c>
       <c r="C67" t="n">
-        <v>308.075</v>
+        <v>272.9599999999988</v>
       </c>
     </row>
     <row r="68">
@@ -2094,7 +1919,7 @@
         <v>2</v>
       </c>
       <c r="C68" t="n">
-        <v>318.99</v>
+        <v>283.2849999999988</v>
       </c>
     </row>
     <row r="69">
@@ -2105,7 +1930,7 @@
         <v>3</v>
       </c>
       <c r="C69" t="n">
-        <v>312.23</v>
+        <v>256.7699999999988</v>
       </c>
     </row>
     <row r="70">
@@ -2116,7 +1941,7 @@
         <v>4</v>
       </c>
       <c r="C70" t="n">
-        <v>322.11</v>
+        <v>275.9449999999989</v>
       </c>
     </row>
     <row r="71">
@@ -2127,7 +1952,7 @@
         <v>5</v>
       </c>
       <c r="C71" t="n">
-        <v>305.64</v>
+        <v>263.9099999999988</v>
       </c>
     </row>
   </sheetData>
@@ -2229,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>32.51499999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -2240,7 +2065,7 @@
         <v>2</v>
       </c>
       <c r="C8" t="n">
-        <v>52.86000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -2251,7 +2076,7 @@
         <v>3</v>
       </c>
       <c r="C9" t="n">
-        <v>31.56999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -2262,7 +2087,7 @@
         <v>4</v>
       </c>
       <c r="C10" t="n">
-        <v>43.88999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -2273,7 +2098,7 @@
         <v>5</v>
       </c>
       <c r="C11" t="n">
-        <v>36.81999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -2284,7 +2109,7 @@
         <v>1</v>
       </c>
       <c r="C12" t="n">
-        <v>33.075</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -2295,7 +2120,7 @@
         <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>43.99</v>
+        <v>8.284999999998837</v>
       </c>
     </row>
     <row r="14">
@@ -2306,7 +2131,7 @@
         <v>3</v>
       </c>
       <c r="C14" t="n">
-        <v>37.23</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -2317,7 +2142,7 @@
         <v>4</v>
       </c>
       <c r="C15" t="n">
-        <v>47.11</v>
+        <v>0.9449999999988359</v>
       </c>
     </row>
     <row r="16">
@@ -2328,7 +2153,7 @@
         <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>30.64</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2375,7 +2200,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>12.775</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -2386,7 +2211,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>18.32</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2397,7 +2222,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>13.155</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2408,7 +2233,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>20.115</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2419,7 +2244,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>17.825</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2928,7 +2753,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2955,10 +2780,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
@@ -2966,100 +2791,12 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
-      <c r="C5" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>2</v>
-      </c>
-      <c r="B6" t="n">
-        <v>5</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>5</v>
-      </c>
-      <c r="B8" t="n">
-        <v>2</v>
-      </c>
-      <c r="C8" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>5</v>
-      </c>
-      <c r="B9" t="n">
-        <v>3</v>
-      </c>
-      <c r="C9" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>5</v>
-      </c>
-      <c r="B10" t="n">
-        <v>4</v>
-      </c>
-      <c r="C10" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>5</v>
-      </c>
-      <c r="B11" t="n">
-        <v>5</v>
-      </c>
-      <c r="C11" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>